<commit_message>
incluimos histórico de jornadas
</commit_message>
<xml_diff>
--- a/data_in/Resultados futbol matías.xlsx
+++ b/data_in/Resultados futbol matías.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milen\Desktop\git\futbol_m\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9266B03C-A620-4C09-B4CB-60348A3487E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7904E5BD-9ACD-417C-B81C-D2C1C1079825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27930" windowHeight="16440" activeTab="3" xr2:uid="{08B94FEF-8F58-4A5E-B536-4E4CD1DEF899}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27930" windowHeight="16440" activeTab="29" xr2:uid="{08B94FEF-8F58-4A5E-B536-4E4CD1DEF899}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 9" sheetId="31" r:id="rId1"/>
@@ -43,7 +43,6 @@
     <sheet name="Table 10" sheetId="4" r:id="rId28"/>
     <sheet name="Table 1" sheetId="3" r:id="rId29"/>
     <sheet name="Table 0" sheetId="2" r:id="rId30"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId31"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="29" hidden="1">'Table 0'!$A$1:$G$9</definedName>
@@ -2034,13 +2033,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{6A798592-7ED7-411E-93BE-5DD7BBA7DFC3}" name="Table_9" displayName="Table_9" ref="A1:G9" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G9" xr:uid="{6A798592-7ED7-411E-93BE-5DD7BBA7DFC3}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{47AC6AE4-AF51-424D-BC77-C9349EF6D905}" uniqueName="1" name="Jornada 10" queryTableFieldId="1" dataDxfId="187"/>
-    <tableColumn id="2" xr3:uid="{5652BEB4-FAB8-4690-AB71-547E69A2DF01}" uniqueName="2" name="Jornada 102" queryTableFieldId="2" dataDxfId="186"/>
-    <tableColumn id="3" xr3:uid="{1EF15115-9E42-4A31-BED9-CE1CDE39C94D}" uniqueName="3" name="Jornada 103" queryTableFieldId="3" dataDxfId="185"/>
-    <tableColumn id="4" xr3:uid="{742121A5-7B41-4C80-A871-CD8179460D7D}" uniqueName="4" name="Jornada 104" queryTableFieldId="4" dataDxfId="184"/>
-    <tableColumn id="5" xr3:uid="{D12DF7A3-6C73-4B81-B6D6-F4EA4D4BAC11}" uniqueName="5" name="18-12-2022" queryTableFieldId="5" dataDxfId="183"/>
-    <tableColumn id="6" xr3:uid="{33F7D21E-6604-4522-9506-3E0266D78A0E}" uniqueName="6" name="18-12-20222" queryTableFieldId="6" dataDxfId="182"/>
-    <tableColumn id="7" xr3:uid="{E619B802-C05C-4CE6-AEF0-580589E64F6F}" uniqueName="7" name="18-12-20223" queryTableFieldId="7" dataDxfId="181"/>
+    <tableColumn id="1" xr3:uid="{47AC6AE4-AF51-424D-BC77-C9349EF6D905}" uniqueName="1" name="Jornada 10" queryTableFieldId="1" dataDxfId="199"/>
+    <tableColumn id="2" xr3:uid="{5652BEB4-FAB8-4690-AB71-547E69A2DF01}" uniqueName="2" name="Jornada 102" queryTableFieldId="2" dataDxfId="198"/>
+    <tableColumn id="3" xr3:uid="{1EF15115-9E42-4A31-BED9-CE1CDE39C94D}" uniqueName="3" name="Jornada 103" queryTableFieldId="3" dataDxfId="197"/>
+    <tableColumn id="4" xr3:uid="{742121A5-7B41-4C80-A871-CD8179460D7D}" uniqueName="4" name="Jornada 104" queryTableFieldId="4" dataDxfId="196"/>
+    <tableColumn id="5" xr3:uid="{D12DF7A3-6C73-4B81-B6D6-F4EA4D4BAC11}" uniqueName="5" name="18-12-2022" queryTableFieldId="5" dataDxfId="195"/>
+    <tableColumn id="6" xr3:uid="{33F7D21E-6604-4522-9506-3E0266D78A0E}" uniqueName="6" name="18-12-20222" queryTableFieldId="6" dataDxfId="194"/>
+    <tableColumn id="7" xr3:uid="{E619B802-C05C-4CE6-AEF0-580589E64F6F}" uniqueName="7" name="18-12-20223" queryTableFieldId="7" dataDxfId="193"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2210,13 +2209,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{564AF572-73E4-4F8C-B149-D0D6EC20D82C}" name="Table_8" displayName="Table_8" ref="A1:G9" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G9" xr:uid="{564AF572-73E4-4F8C-B149-D0D6EC20D82C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F8CAD5D0-524D-41D0-9770-7D757C3A0966}" uniqueName="1" name="Jornada 9" queryTableFieldId="1" dataDxfId="194"/>
-    <tableColumn id="2" xr3:uid="{E599BA6D-BF0B-40C4-83FF-3EB723E2AB60}" uniqueName="2" name="Jornada 92" queryTableFieldId="2" dataDxfId="193"/>
-    <tableColumn id="3" xr3:uid="{8FEA123C-432B-4C2E-9625-56275D319A35}" uniqueName="3" name="Jornada 93" queryTableFieldId="3" dataDxfId="192"/>
-    <tableColumn id="4" xr3:uid="{5C8985D7-6127-4C0D-BED7-26A3299DD914}" uniqueName="4" name="Jornada 94" queryTableFieldId="4" dataDxfId="191"/>
-    <tableColumn id="5" xr3:uid="{FF6AEA84-2A1F-4228-8DCD-5E2BBC7D24DD}" uniqueName="5" name="11-12-2022" queryTableFieldId="5" dataDxfId="190"/>
-    <tableColumn id="6" xr3:uid="{4BBD9DDC-F4BD-4778-B612-0A4F6C32E75D}" uniqueName="6" name="11-12-20222" queryTableFieldId="6" dataDxfId="189"/>
-    <tableColumn id="7" xr3:uid="{E36D6BF0-5C96-4145-AE18-6DD242E3C616}" uniqueName="7" name="11-12-20223" queryTableFieldId="7" dataDxfId="188"/>
+    <tableColumn id="1" xr3:uid="{F8CAD5D0-524D-41D0-9770-7D757C3A0966}" uniqueName="1" name="Jornada 9" queryTableFieldId="1" dataDxfId="192"/>
+    <tableColumn id="2" xr3:uid="{E599BA6D-BF0B-40C4-83FF-3EB723E2AB60}" uniqueName="2" name="Jornada 92" queryTableFieldId="2" dataDxfId="191"/>
+    <tableColumn id="3" xr3:uid="{8FEA123C-432B-4C2E-9625-56275D319A35}" uniqueName="3" name="Jornada 93" queryTableFieldId="3" dataDxfId="190"/>
+    <tableColumn id="4" xr3:uid="{5C8985D7-6127-4C0D-BED7-26A3299DD914}" uniqueName="4" name="Jornada 94" queryTableFieldId="4" dataDxfId="189"/>
+    <tableColumn id="5" xr3:uid="{FF6AEA84-2A1F-4228-8DCD-5E2BBC7D24DD}" uniqueName="5" name="11-12-2022" queryTableFieldId="5" dataDxfId="188"/>
+    <tableColumn id="6" xr3:uid="{4BBD9DDC-F4BD-4778-B612-0A4F6C32E75D}" uniqueName="6" name="11-12-20222" queryTableFieldId="6" dataDxfId="187"/>
+    <tableColumn id="7" xr3:uid="{E36D6BF0-5C96-4145-AE18-6DD242E3C616}" uniqueName="7" name="11-12-20223" queryTableFieldId="7" dataDxfId="186"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2386,13 +2385,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{47AE3A60-702A-4555-85F9-4F7AE067B145}" name="Table_7" displayName="Table_7" ref="A1:G9" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G9" xr:uid="{47AE3A60-702A-4555-85F9-4F7AE067B145}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{E982C2F9-B98F-49A9-BFC4-CBF30CF867FF}" uniqueName="1" name="Jornada 8" queryTableFieldId="1" dataDxfId="180"/>
-    <tableColumn id="2" xr3:uid="{F19A3147-05EB-45A5-9BF6-DB9A06AFCF2D}" uniqueName="2" name="Jornada 82" queryTableFieldId="2" dataDxfId="179"/>
-    <tableColumn id="3" xr3:uid="{563E2A67-FC9D-4D9D-8E76-8B9AA0114BC5}" uniqueName="3" name="Jornada 83" queryTableFieldId="3" dataDxfId="178"/>
-    <tableColumn id="4" xr3:uid="{8FE2BA31-A624-49C1-AE6C-C2FD8EDC225C}" uniqueName="4" name="Jornada 84" queryTableFieldId="4" dataDxfId="177"/>
-    <tableColumn id="5" xr3:uid="{946E96E1-4FAA-4EAF-8A65-BF7E5C2A38DE}" uniqueName="5" name="27-11-2022" queryTableFieldId="5" dataDxfId="176"/>
-    <tableColumn id="6" xr3:uid="{A39766CD-FA2A-4DFB-B1FA-AE942D588FA1}" uniqueName="6" name="27-11-20222" queryTableFieldId="6" dataDxfId="175"/>
-    <tableColumn id="7" xr3:uid="{9A7884DF-9569-48E3-A918-7ED88403AD6B}" uniqueName="7" name="27-11-20223" queryTableFieldId="7" dataDxfId="174"/>
+    <tableColumn id="1" xr3:uid="{E982C2F9-B98F-49A9-BFC4-CBF30CF867FF}" uniqueName="1" name="Jornada 8" queryTableFieldId="1" dataDxfId="185"/>
+    <tableColumn id="2" xr3:uid="{F19A3147-05EB-45A5-9BF6-DB9A06AFCF2D}" uniqueName="2" name="Jornada 82" queryTableFieldId="2" dataDxfId="184"/>
+    <tableColumn id="3" xr3:uid="{563E2A67-FC9D-4D9D-8E76-8B9AA0114BC5}" uniqueName="3" name="Jornada 83" queryTableFieldId="3" dataDxfId="183"/>
+    <tableColumn id="4" xr3:uid="{8FE2BA31-A624-49C1-AE6C-C2FD8EDC225C}" uniqueName="4" name="Jornada 84" queryTableFieldId="4" dataDxfId="182"/>
+    <tableColumn id="5" xr3:uid="{946E96E1-4FAA-4EAF-8A65-BF7E5C2A38DE}" uniqueName="5" name="27-11-2022" queryTableFieldId="5" dataDxfId="181"/>
+    <tableColumn id="6" xr3:uid="{A39766CD-FA2A-4DFB-B1FA-AE942D588FA1}" uniqueName="6" name="27-11-20222" queryTableFieldId="6" dataDxfId="180"/>
+    <tableColumn id="7" xr3:uid="{9A7884DF-9569-48E3-A918-7ED88403AD6B}" uniqueName="7" name="27-11-20223" queryTableFieldId="7" dataDxfId="179"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2418,13 +2417,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{7538B651-E7FE-47AA-9950-9A25C53449E7}" name="Table_6" displayName="Table_6" ref="A1:G9" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G9" xr:uid="{7538B651-E7FE-47AA-9950-9A25C53449E7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1CBC4379-3177-41DF-8A1E-C6E2D6D60DE3}" uniqueName="1" name="Jornada 7" queryTableFieldId="1" dataDxfId="173"/>
-    <tableColumn id="2" xr3:uid="{78870B1E-EC36-40A1-8C79-67C7BCA48BC6}" uniqueName="2" name="Jornada 72" queryTableFieldId="2" dataDxfId="172"/>
-    <tableColumn id="3" xr3:uid="{209BDBF1-1248-40EF-88E3-57F07D922EC3}" uniqueName="3" name="Jornada 73" queryTableFieldId="3" dataDxfId="171"/>
-    <tableColumn id="4" xr3:uid="{EB92EFCB-8654-4461-AB7B-2B1C64BBCA4F}" uniqueName="4" name="Jornada 74" queryTableFieldId="4" dataDxfId="170"/>
-    <tableColumn id="5" xr3:uid="{B3D7DEF4-3BF3-4732-B487-357AC5A4EA57}" uniqueName="5" name="20-11-2022" queryTableFieldId="5" dataDxfId="169"/>
-    <tableColumn id="6" xr3:uid="{4A63BC11-FA52-43EA-9730-BDACBBC29AC8}" uniqueName="6" name="20-11-20222" queryTableFieldId="6" dataDxfId="168"/>
-    <tableColumn id="7" xr3:uid="{F7C7493A-8A1B-411B-B53C-9BA9851419CB}" uniqueName="7" name="20-11-20223" queryTableFieldId="7" dataDxfId="167"/>
+    <tableColumn id="1" xr3:uid="{1CBC4379-3177-41DF-8A1E-C6E2D6D60DE3}" uniqueName="1" name="Jornada 7" queryTableFieldId="1" dataDxfId="178"/>
+    <tableColumn id="2" xr3:uid="{78870B1E-EC36-40A1-8C79-67C7BCA48BC6}" uniqueName="2" name="Jornada 72" queryTableFieldId="2" dataDxfId="177"/>
+    <tableColumn id="3" xr3:uid="{209BDBF1-1248-40EF-88E3-57F07D922EC3}" uniqueName="3" name="Jornada 73" queryTableFieldId="3" dataDxfId="176"/>
+    <tableColumn id="4" xr3:uid="{EB92EFCB-8654-4461-AB7B-2B1C64BBCA4F}" uniqueName="4" name="Jornada 74" queryTableFieldId="4" dataDxfId="175"/>
+    <tableColumn id="5" xr3:uid="{B3D7DEF4-3BF3-4732-B487-357AC5A4EA57}" uniqueName="5" name="20-11-2022" queryTableFieldId="5" dataDxfId="174"/>
+    <tableColumn id="6" xr3:uid="{4A63BC11-FA52-43EA-9730-BDACBBC29AC8}" uniqueName="6" name="20-11-20222" queryTableFieldId="6" dataDxfId="173"/>
+    <tableColumn id="7" xr3:uid="{F7C7493A-8A1B-411B-B53C-9BA9851419CB}" uniqueName="7" name="20-11-20223" queryTableFieldId="7" dataDxfId="172"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2434,13 +2433,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{717B277B-55E5-47DE-80C1-78223F53E3F8}" name="Table_5" displayName="Table_5" ref="A1:G9" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G9" xr:uid="{717B277B-55E5-47DE-80C1-78223F53E3F8}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{87242D49-9F9D-4381-A2A7-C346A8D021C0}" uniqueName="1" name="Jornada 6" queryTableFieldId="1" dataDxfId="199"/>
-    <tableColumn id="2" xr3:uid="{9CE0B498-BB6B-4511-9026-09241E27224A}" uniqueName="2" name="Jornada 62" queryTableFieldId="2" dataDxfId="198"/>
+    <tableColumn id="1" xr3:uid="{87242D49-9F9D-4381-A2A7-C346A8D021C0}" uniqueName="1" name="Jornada 6" queryTableFieldId="1" dataDxfId="171"/>
+    <tableColumn id="2" xr3:uid="{9CE0B498-BB6B-4511-9026-09241E27224A}" uniqueName="2" name="Jornada 62" queryTableFieldId="2" dataDxfId="170"/>
     <tableColumn id="3" xr3:uid="{A4333C07-F45F-4D14-9A09-98AC58568A32}" uniqueName="3" name="Jornada 63" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{F0D50705-C14B-4131-80E4-7B9EC699F776}" uniqueName="4" name="Jornada 64" queryTableFieldId="4" dataDxfId="197"/>
+    <tableColumn id="4" xr3:uid="{F0D50705-C14B-4131-80E4-7B9EC699F776}" uniqueName="4" name="Jornada 64" queryTableFieldId="4" dataDxfId="169"/>
     <tableColumn id="5" xr3:uid="{B96039C6-5A38-431B-9350-5B9F729BE9A9}" uniqueName="5" name="13-11-2022" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{655F0ECA-6584-495D-B168-3AFD982D42F2}" uniqueName="6" name="13-11-20222" queryTableFieldId="6" dataDxfId="196"/>
-    <tableColumn id="7" xr3:uid="{F53A6275-27DE-422E-9408-242E833CC5F0}" uniqueName="7" name="13-11-20223" queryTableFieldId="7" dataDxfId="195"/>
+    <tableColumn id="6" xr3:uid="{655F0ECA-6584-495D-B168-3AFD982D42F2}" uniqueName="6" name="13-11-20222" queryTableFieldId="6" dataDxfId="168"/>
+    <tableColumn id="7" xr3:uid="{F53A6275-27DE-422E-9408-242E833CC5F0}" uniqueName="7" name="13-11-20223" queryTableFieldId="7" dataDxfId="167"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7433,7 +7432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EDCA9DA-2382-4622-B3AB-3DB19ED780B7}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -7659,23 +7658,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFAAF097-AD91-4939-B5B3-7E2F6BCE0683}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7EDBB7-8E79-4377-B2BB-071B3EA518A3}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>

</xml_diff>